<commit_message>
cleaned up all scripts
Made 'df' concistent as 'so279_df' throughout all scripts + format cleanup
</commit_message>
<xml_diff>
--- a/data/stations_coordinates.xlsx
+++ b/data/stations_coordinates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_GITHUB/NAPTRAM2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{9489D397-5F77-4F7E-BFDB-5CBC5D09A5CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EF0BB4B0-1A94-4FA1-BCA7-E4B7FCF27AE7}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{9489D397-5F77-4F7E-BFDB-5CBC5D09A5CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{69EC6F2E-FF74-4501-88FF-39F3BC36701C}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="7360" xr2:uid="{61907058-4423-48CC-A770-F64096544107}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{61907058-4423-48CC-A770-F64096544107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,10 +87,10 @@
     <t>lon_deg</t>
   </si>
   <si>
-    <t>lat_dec</t>
-  </si>
-  <si>
-    <t>lon_dec</t>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lon</t>
   </si>
 </sst>
 </file>
@@ -445,16 +445,16 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +471,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -488,7 +488,7 @@
         <v>-10.1075</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -505,7 +505,7 @@
         <v>-24.820277999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -522,7 +522,7 @@
         <v>-29.323333000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -539,7 +539,7 @@
         <v>-33.826943999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -556,7 +556,7 @@
         <v>-34.497222000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -573,7 +573,7 @@
         <v>-33.785556</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>

</xml_diff>